<commit_message>
Update 16 Jan 2023
</commit_message>
<xml_diff>
--- a/data_supp/Database Area untuk Report.xlsx
+++ b/data_supp/Database Area untuk Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.nathanael\Documents\Python\Data\2. Master Data Git\data_supp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708CC534-82E0-4785-9AEF-FC5DBF0660B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3464DA6-3647-4CD9-92DF-5FDE786BACD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CB92B276-28E0-4829-B796-ADBF995E2FE3}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="127">
   <si>
     <t>City</t>
   </si>
@@ -411,13 +411,22 @@
   </si>
   <si>
     <t>Gorontalo Province</t>
+  </si>
+  <si>
+    <t>West Sulawesi Province</t>
+  </si>
+  <si>
+    <t>Riau islands</t>
+  </si>
+  <si>
+    <t>West Nusa Tenggara Province</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -816,7 +825,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -824,19 +833,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{904F3AA4-01F5-4399-A1EE-4BB38BAA3B9E}">
-  <dimension ref="A1:B112"/>
+  <dimension ref="A1:B115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B113" sqref="B113"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B119" sqref="B119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27.08984375" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -844,7 +853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
@@ -852,7 +861,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>41</v>
       </c>
@@ -860,7 +869,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>42</v>
       </c>
@@ -868,7 +877,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>43</v>
       </c>
@@ -876,7 +885,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>44</v>
       </c>
@@ -884,7 +893,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>96</v>
       </c>
@@ -892,7 +901,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>108</v>
       </c>
@@ -900,7 +909,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>111</v>
       </c>
@@ -908,7 +917,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -916,7 +925,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
@@ -924,7 +933,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
@@ -932,7 +941,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
@@ -940,7 +949,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -948,7 +957,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
@@ -956,7 +965,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>10</v>
       </c>
@@ -964,7 +973,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>11</v>
       </c>
@@ -972,7 +981,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>12</v>
       </c>
@@ -980,7 +989,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>13</v>
       </c>
@@ -988,7 +997,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>14</v>
       </c>
@@ -996,7 +1005,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>15</v>
       </c>
@@ -1004,7 +1013,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>16</v>
       </c>
@@ -1012,7 +1021,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>17</v>
       </c>
@@ -1020,7 +1029,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>18</v>
       </c>
@@ -1028,7 +1037,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>19</v>
       </c>
@@ -1036,7 +1045,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -1044,7 +1053,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -1052,7 +1061,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -1060,7 +1069,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>64</v>
       </c>
@@ -1068,7 +1077,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -1076,7 +1085,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>72</v>
       </c>
@@ -1084,7 +1093,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>74</v>
       </c>
@@ -1092,7 +1101,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>80</v>
       </c>
@@ -1100,7 +1109,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>101</v>
       </c>
@@ -1108,7 +1117,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>3</v>
       </c>
@@ -1116,7 +1125,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>73</v>
       </c>
@@ -1124,7 +1133,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>78</v>
       </c>
@@ -1132,7 +1141,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>25</v>
       </c>
@@ -1140,7 +1149,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>28</v>
       </c>
@@ -1148,7 +1157,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>65</v>
       </c>
@@ -1156,7 +1165,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="8" t="s">
         <v>77</v>
       </c>
@@ -1164,7 +1173,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>79</v>
       </c>
@@ -1172,7 +1181,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>85</v>
       </c>
@@ -1180,7 +1189,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>92</v>
       </c>
@@ -1188,7 +1197,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>29</v>
       </c>
@@ -1196,7 +1205,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>71</v>
       </c>
@@ -1204,7 +1213,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>76</v>
       </c>
@@ -1212,7 +1221,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>30</v>
       </c>
@@ -1220,7 +1229,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>31</v>
       </c>
@@ -1228,7 +1237,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>32</v>
       </c>
@@ -1236,7 +1245,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>33</v>
       </c>
@@ -1244,7 +1253,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>34</v>
       </c>
@@ -1252,7 +1261,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
         <v>83</v>
       </c>
@@ -1260,7 +1269,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
         <v>84</v>
       </c>
@@ -1268,7 +1277,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="10" t="s">
         <v>88</v>
       </c>
@@ -1276,7 +1285,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>98</v>
       </c>
@@ -1284,7 +1293,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="10" t="s">
         <v>104</v>
       </c>
@@ -1292,7 +1301,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
         <v>105</v>
       </c>
@@ -1300,7 +1309,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>38</v>
       </c>
@@ -1308,7 +1317,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>39</v>
       </c>
@@ -1316,7 +1325,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>45</v>
       </c>
@@ -1324,7 +1333,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>46</v>
       </c>
@@ -1332,7 +1341,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
         <v>100</v>
       </c>
@@ -1340,7 +1349,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>26</v>
       </c>
@@ -1348,7 +1357,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>48</v>
       </c>
@@ -1356,7 +1365,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>49</v>
       </c>
@@ -1364,7 +1373,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>50</v>
       </c>
@@ -1372,7 +1381,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>51</v>
       </c>
@@ -1380,7 +1389,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>52</v>
       </c>
@@ -1388,7 +1397,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
         <v>82</v>
       </c>
@@ -1396,7 +1405,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="5" t="s">
         <v>87</v>
       </c>
@@ -1404,7 +1413,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
         <v>93</v>
       </c>
@@ -1412,7 +1421,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
         <v>99</v>
       </c>
@@ -1420,7 +1429,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" s="5" t="s">
         <v>102</v>
       </c>
@@ -1428,7 +1437,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
         <v>107</v>
       </c>
@@ -1436,7 +1445,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
         <v>110</v>
       </c>
@@ -1444,7 +1453,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>21</v>
       </c>
@@ -1452,7 +1461,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>36</v>
       </c>
@@ -1460,7 +1469,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>40</v>
       </c>
@@ -1468,7 +1477,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>47</v>
       </c>
@@ -1476,7 +1485,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>53</v>
       </c>
@@ -1484,7 +1493,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>55</v>
       </c>
@@ -1492,7 +1501,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
         <v>75</v>
       </c>
@@ -1500,7 +1509,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
         <v>81</v>
       </c>
@@ -1508,7 +1517,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
         <v>89</v>
       </c>
@@ -1516,7 +1525,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
         <v>90</v>
       </c>
@@ -1524,7 +1533,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
         <v>91</v>
       </c>
@@ -1532,7 +1541,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
         <v>97</v>
       </c>
@@ -1540,7 +1549,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
         <v>103</v>
       </c>
@@ -1548,7 +1557,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
         <v>106</v>
       </c>
@@ -1556,7 +1565,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>23</v>
       </c>
@@ -1564,7 +1573,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>24</v>
       </c>
@@ -1572,7 +1581,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>27</v>
       </c>
@@ -1580,7 +1589,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>35</v>
       </c>
@@ -1588,7 +1597,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>37</v>
       </c>
@@ -1596,7 +1605,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>54</v>
       </c>
@@ -1604,7 +1613,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" s="5" t="s">
         <v>86</v>
       </c>
@@ -1612,7 +1621,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" s="5" t="s">
         <v>94</v>
       </c>
@@ -1620,7 +1629,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" s="5" t="s">
         <v>95</v>
       </c>
@@ -1628,7 +1637,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" s="5" t="s">
         <v>109</v>
       </c>
@@ -1636,7 +1645,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" s="5" t="s">
         <v>112</v>
       </c>
@@ -1644,7 +1653,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
         <v>113</v>
       </c>
@@ -1652,7 +1661,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" s="5" t="s">
         <v>114</v>
       </c>
@@ -1660,7 +1669,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" s="5" t="s">
         <v>115</v>
       </c>
@@ -1668,7 +1677,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" s="5" t="s">
         <v>116</v>
       </c>
@@ -1676,7 +1685,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" s="5" t="s">
         <v>117</v>
       </c>
@@ -1684,7 +1693,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" s="5" t="s">
         <v>118</v>
       </c>
@@ -1692,7 +1701,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" s="5" t="s">
         <v>119</v>
       </c>
@@ -1700,7 +1709,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" s="5" t="s">
         <v>120</v>
       </c>
@@ -1708,7 +1717,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" s="5" t="s">
         <v>121</v>
       </c>
@@ -1716,7 +1725,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" s="5" t="s">
         <v>122</v>
       </c>
@@ -1724,12 +1733,36 @@
         <v>59</v>
       </c>
     </row>
-    <row r="112" spans="1:2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" s="5" t="s">
         <v>123</v>
       </c>
       <c r="B112" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A113" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B113" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B114" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A115" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B115" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1751,13 +1784,13 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.08984375" customWidth="1"/>
     <col min="6" max="6" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -1766,7 +1799,7 @@
       </c>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1775,7 +1808,7 @@
       </c>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1784,7 +1817,7 @@
       </c>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1793,7 +1826,7 @@
       </c>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1802,7 +1835,7 @@
       </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>65</v>
       </c>
@@ -1811,7 +1844,7 @@
       </c>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -1820,7 +1853,7 @@
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1829,7 +1862,7 @@
       </c>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1838,7 +1871,7 @@
       </c>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1847,7 +1880,7 @@
       </c>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1856,7 +1889,7 @@
       </c>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1865,7 +1898,7 @@
       </c>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1874,7 +1907,7 @@
       </c>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -1883,7 +1916,7 @@
       </c>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1892,7 +1925,7 @@
       </c>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1901,7 +1934,7 @@
       </c>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1910,7 +1943,7 @@
       </c>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1919,7 +1952,7 @@
       </c>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1928,7 +1961,7 @@
       </c>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1937,7 +1970,7 @@
       </c>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -1946,7 +1979,7 @@
       </c>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -1955,7 +1988,7 @@
       </c>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -1964,7 +1997,7 @@
       </c>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -1973,7 +2006,7 @@
       </c>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -1982,7 +2015,7 @@
       </c>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>44</v>
       </c>
@@ -1991,7 +2024,7 @@
       </c>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -2000,7 +2033,7 @@
       </c>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -2009,7 +2042,7 @@
       </c>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -2018,7 +2051,7 @@
       </c>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -2027,7 +2060,7 @@
       </c>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -2036,7 +2069,7 @@
       </c>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>50</v>
       </c>
@@ -2045,7 +2078,7 @@
       </c>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -2054,7 +2087,7 @@
       </c>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -2063,7 +2096,7 @@
       </c>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>53</v>
       </c>
@@ -2072,7 +2105,7 @@
       </c>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>54</v>
       </c>
@@ -2081,7 +2114,7 @@
       </c>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>55</v>
       </c>

</xml_diff>